<commit_message>
manuscript updates and readme file updates for iso data
</commit_message>
<xml_diff>
--- a/doc/manuscript/Tables.xlsx
+++ b/doc/manuscript/Tables.xlsx
@@ -4,16 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="0" windowWidth="25120" windowHeight="15640" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="140" yWindow="0" windowWidth="21680" windowHeight="15220" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="4" r:id="rId1"/>
     <sheet name="Table1" sheetId="1" r:id="rId2"/>
-    <sheet name="Table2" sheetId="2" r:id="rId3"/>
-    <sheet name="Table3" sheetId="3" r:id="rId4"/>
+    <sheet name="Table1-2" sheetId="5" r:id="rId3"/>
+    <sheet name="Table2" sheetId="2" r:id="rId4"/>
+    <sheet name="Table3" sheetId="3" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="122">
   <si>
     <t>Experiment 1</t>
   </si>
@@ -287,9 +288,6 @@
   </si>
   <si>
     <t>Walker Branch, TN</t>
-  </si>
-  <si>
-    <t>Initial laboratory</t>
   </si>
   <si>
     <t>UCI</t>
@@ -408,6 +406,48 @@
   <si>
     <t>period</t>
   </si>
+  <si>
+    <t>experiment</t>
+  </si>
+  <si>
+    <t>sample collection date</t>
+  </si>
+  <si>
+    <t>% water holding capacity</t>
+  </si>
+  <si>
+    <t>initial moisture content*</t>
+  </si>
+  <si>
+    <t>* mean field moisture content for control samples (n = 12 for Experiment 1, n = 6 for Experiment 2); air-dry moisture content for treatment samples</t>
+  </si>
+  <si>
+    <r>
+      <t>∆</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>C measured</t>
+    </r>
+  </si>
+  <si>
+    <t>Control incubation laboratory</t>
+  </si>
 </sst>
 </file>
 
@@ -417,7 +457,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -522,19 +562,18 @@
       <name val="Cambria"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Cambria"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -564,7 +603,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="167">
+  <cellStyleXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -732,8 +771,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -781,24 +854,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -808,9 +863,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -842,8 +894,42 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="167">
+  <cellStyles count="201">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -927,6 +1013,23 @@
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1010,6 +1113,23 @@
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3177,8 +3297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I19" sqref="A4:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3195,365 +3315,365 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="25"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" ht="20">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="20">
         <v>2011</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28" t="s">
+      <c r="G5" s="33"/>
+      <c r="H5" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="28"/>
+      <c r="I5" s="33"/>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="G6" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" customHeight="1">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="24"/>
+    </row>
+    <row r="8" spans="1:9" ht="5" customHeight="1">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="27">
+        <v>2011</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="27">
+        <v>60</v>
+      </c>
+      <c r="E9" s="27">
+        <v>20</v>
+      </c>
+      <c r="F9" s="27">
+        <v>4</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="27">
+        <v>14</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16" customHeight="1">
+      <c r="A10" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="28">
+        <v>2018</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="28">
+        <v>60</v>
+      </c>
+      <c r="E10" s="28">
+        <v>20</v>
+      </c>
+      <c r="F10" s="28">
+        <v>4</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+    </row>
+    <row r="12" spans="1:9" ht="20">
+      <c r="A12" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="20">
+        <v>2019</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="33"/>
+    </row>
+    <row r="15" spans="1:9" s="5" customFormat="1" ht="30" customHeight="1">
+      <c r="A15" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="H6" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="I6" s="30" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" customHeight="1">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31" t="s">
+      <c r="F15" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="30" customFormat="1" ht="30" customHeight="1">
+      <c r="A16" s="21"/>
+      <c r="B16" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="33" t="s">
+      <c r="C16" s="25"/>
+      <c r="D16" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E16" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F16" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31" t="s">
+      <c r="G16" s="24"/>
+      <c r="H16" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="31"/>
-    </row>
-    <row r="8" spans="1:9" ht="5" customHeight="1">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="34" t="s">
+      <c r="I16" s="24"/>
+    </row>
+    <row r="17" spans="1:9" s="30" customFormat="1" ht="5" customHeight="1">
+      <c r="A17" s="21"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+    </row>
+    <row r="18" spans="1:9" ht="20" customHeight="1">
+      <c r="A18" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="34">
-        <v>2011</v>
-      </c>
-      <c r="C9" s="34" t="s">
+      <c r="B18" s="27">
+        <v>2019</v>
+      </c>
+      <c r="C18" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D18" s="27">
         <v>60</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E18" s="27">
         <v>20</v>
       </c>
-      <c r="F9" s="34">
+      <c r="F18" s="27">
         <v>4</v>
       </c>
-      <c r="G9" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="34">
-        <v>14</v>
-      </c>
-      <c r="I9" s="34" t="s">
+      <c r="G18" s="27" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="16" customHeight="1">
-      <c r="A10" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="35">
-        <v>2018</v>
-      </c>
-      <c r="C10" s="35" t="s">
+      <c r="H18" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="35">
+    </row>
+    <row r="19" spans="1:9" ht="16" customHeight="1">
+      <c r="A19" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="28">
+        <v>2019</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="28">
         <v>60</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E19" s="28">
         <v>20</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F19" s="28">
         <v>4</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G19" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="35" t="s">
+      <c r="H19" s="28">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-    </row>
-    <row r="12" spans="1:9" ht="20">
-      <c r="A12" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="26">
-        <v>2019</v>
-      </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="28"/>
-    </row>
-    <row r="15" spans="1:9" s="5" customFormat="1" ht="30" customHeight="1">
-      <c r="A15" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="G15" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="H15" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="I15" s="30" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="37" customFormat="1" ht="30" customHeight="1">
-      <c r="A16" s="27"/>
-      <c r="B16" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="I16" s="31"/>
-    </row>
-    <row r="17" spans="1:9" s="37" customFormat="1" ht="5" customHeight="1">
-      <c r="A17" s="27"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-    </row>
-    <row r="18" spans="1:9" ht="20" customHeight="1">
-      <c r="A18" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="34">
-        <v>2019</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="34">
-        <v>60</v>
-      </c>
-      <c r="E18" s="34">
-        <v>20</v>
-      </c>
-      <c r="F18" s="34">
-        <v>4</v>
-      </c>
-      <c r="G18" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="16" customHeight="1">
-      <c r="A19" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="35">
-        <v>2019</v>
-      </c>
-      <c r="C19" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="35">
-        <v>60</v>
-      </c>
-      <c r="E19" s="35">
-        <v>20</v>
-      </c>
-      <c r="F19" s="35">
-        <v>4</v>
-      </c>
-      <c r="G19" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="35">
-        <v>7</v>
-      </c>
-      <c r="I19" s="35" t="s">
+      <c r="I19" s="28" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3578,10 +3698,270 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A2:J10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="33"/>
+    </row>
+    <row r="4" spans="1:10" ht="45" customHeight="1">
+      <c r="A4" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45" customHeight="1">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="24"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="42">
+        <v>1</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="38">
+        <v>2011</v>
+      </c>
+      <c r="D6" s="38">
+        <v>2011</v>
+      </c>
+      <c r="E6" s="41">
+        <f>AVERAGE(Table2!E6:E17)</f>
+        <v>17.904594562521122</v>
+      </c>
+      <c r="F6" s="38">
+        <v>60</v>
+      </c>
+      <c r="G6" s="38">
+        <v>4</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="38">
+        <v>14</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="42"/>
+      <c r="B7" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="38">
+        <v>2011</v>
+      </c>
+      <c r="D7" s="38">
+        <v>2018</v>
+      </c>
+      <c r="E7" s="41">
+        <v>0</v>
+      </c>
+      <c r="F7" s="38">
+        <v>60</v>
+      </c>
+      <c r="G7" s="38">
+        <v>4</v>
+      </c>
+      <c r="H7" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="42">
+        <v>2</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="38">
+        <v>2019</v>
+      </c>
+      <c r="D8" s="38">
+        <v>2019</v>
+      </c>
+      <c r="E8" s="41">
+        <f>AVERAGE(Table2!F12:F17)</f>
+        <v>18.606574515013019</v>
+      </c>
+      <c r="F8" s="38">
+        <v>60</v>
+      </c>
+      <c r="G8" s="38">
+        <v>4</v>
+      </c>
+      <c r="H8" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="42"/>
+      <c r="B9" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="38">
+        <v>2019</v>
+      </c>
+      <c r="D9" s="38">
+        <v>2019</v>
+      </c>
+      <c r="E9" s="41">
+        <v>0</v>
+      </c>
+      <c r="F9" s="38">
+        <v>60</v>
+      </c>
+      <c r="G9" s="38">
+        <v>4</v>
+      </c>
+      <c r="H9" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="38">
+        <v>7</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3601,17 +3981,17 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="19" t="s">
+      <c r="F2" s="35"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
@@ -3655,10 +4035,10 @@
       <c r="D4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="21"/>
+      <c r="F4" s="36"/>
       <c r="G4" s="2" t="s">
         <v>41</v>
       </c>
@@ -4131,6 +4511,9 @@
         <v>465</v>
       </c>
       <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="E18" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4149,18 +4532,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q66"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" style="1" customWidth="1"/>
@@ -4182,22 +4565,22 @@
       <c r="D2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="14"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
     </row>
     <row r="3" spans="1:17" ht="30">
       <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>77</v>
@@ -4221,12 +4604,12 @@
         <v>49</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="K3" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="L3" s="22"/>
+        <v>110</v>
+      </c>
+      <c r="K3" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="L3" s="37"/>
       <c r="M3" s="4" t="s">
         <v>40</v>
       </c>
@@ -4258,10 +4641,10 @@
         <v>43</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>3</v>
@@ -5313,7 +5696,7 @@
         <v>2009</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" s="10">
         <f>VLOOKUP($G24,[1]Results!$D$2:$L$62,8,FALSE)</f>
@@ -5369,7 +5752,7 @@
         <v>2009</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C25" s="10">
         <f>VLOOKUP($G25,[1]Results!$D$2:$L$62,8,FALSE)</f>
@@ -5425,7 +5808,7 @@
         <v>2009</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C26" s="10">
         <f>VLOOKUP($G26,[1]Results!$D$2:$L$62,8,FALSE)</f>
@@ -5481,7 +5864,7 @@
         <v>2009</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C27" s="10">
         <f>VLOOKUP($G27,[1]Results!$D$2:$L$62,8,FALSE)</f>
@@ -5537,7 +5920,7 @@
         <v>2008</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C28" s="10">
         <f>VLOOKUP($G28,[1]Results!$D$2:$L$62,8,FALSE)</f>
@@ -5572,16 +5955,16 @@
       <c r="N28" s="11">
         <v>0.8</v>
       </c>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="18"/>
+      <c r="O28" s="43"/>
+      <c r="P28" s="43"/>
+      <c r="Q28" s="43"/>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="1">
         <v>2004</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C29" s="10">
         <f>VLOOKUP($G29,[1]Results!$D$2:$L$62,8,FALSE)</f>
@@ -5616,16 +5999,16 @@
       <c r="N29" s="11">
         <v>1.18</v>
       </c>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="18"/>
+      <c r="O29" s="43"/>
+      <c r="P29" s="43"/>
+      <c r="Q29" s="43"/>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="1">
         <v>2004</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C30" s="10">
         <f>VLOOKUP($G30,[1]Results!$D$2:$L$62,8,FALSE)</f>
@@ -5660,16 +6043,16 @@
       <c r="N30" s="11">
         <v>1.18</v>
       </c>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="18"/>
+      <c r="O30" s="43"/>
+      <c r="P30" s="43"/>
+      <c r="Q30" s="43"/>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="1">
         <v>2004</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C31" s="10">
         <f>VLOOKUP($G31,[1]Results!$D$2:$L$62,8,FALSE)</f>
@@ -5704,16 +6087,16 @@
       <c r="N31" s="11">
         <v>1.18</v>
       </c>
-      <c r="O31" s="18"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="18"/>
+      <c r="O31" s="43"/>
+      <c r="P31" s="43"/>
+      <c r="Q31" s="43"/>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="1">
         <v>2004</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C32" s="10">
         <f>VLOOKUP($G32,[1]Results!$D$2:$L$62,8,FALSE)</f>
@@ -5748,16 +6131,16 @@
       <c r="N32" s="11">
         <v>1.18</v>
       </c>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
+      <c r="O32" s="43"/>
+      <c r="P32" s="43"/>
+      <c r="Q32" s="43"/>
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="1">
         <v>2004</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C33" s="10">
         <f>VLOOKUP($G33,[1]Results!$D$2:$L$62,8,FALSE)</f>
@@ -5792,16 +6175,16 @@
       <c r="N33" s="11">
         <v>0.97</v>
       </c>
-      <c r="O33" s="18"/>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="18"/>
+      <c r="O33" s="43"/>
+      <c r="P33" s="43"/>
+      <c r="Q33" s="43"/>
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="1">
         <v>2004</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C34" s="10">
         <f>VLOOKUP($G34,[1]Results!$D$2:$L$62,8,FALSE)</f>
@@ -5836,16 +6219,16 @@
       <c r="N34" s="11">
         <v>0.97</v>
       </c>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
+      <c r="O34" s="43"/>
+      <c r="P34" s="43"/>
+      <c r="Q34" s="43"/>
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="1">
         <v>2004</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C35" s="10">
         <f>VLOOKUP($G35,[1]Results!$D$2:$L$62,8,FALSE)</f>
@@ -5880,16 +6263,16 @@
       <c r="N35" s="11">
         <v>0.97</v>
       </c>
-      <c r="O35" s="18"/>
-      <c r="P35" s="18"/>
-      <c r="Q35" s="18"/>
+      <c r="O35" s="43"/>
+      <c r="P35" s="43"/>
+      <c r="Q35" s="43"/>
     </row>
     <row r="36" spans="1:17">
       <c r="A36" s="1">
         <v>2004</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C36" s="10">
         <f>VLOOKUP($G36,[1]Results!$D$2:$L$62,8,FALSE)</f>
@@ -5924,16 +6307,16 @@
       <c r="N36" s="11">
         <v>0.97</v>
       </c>
-      <c r="O36" s="18"/>
-      <c r="P36" s="18"/>
-      <c r="Q36" s="18"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="43"/>
+      <c r="Q36" s="43"/>
     </row>
     <row r="37" spans="1:17">
       <c r="A37" s="1">
         <v>2004</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C37" s="10">
         <f>VLOOKUP($G37,[1]Results!$D$2:$L$62,8,FALSE)</f>
@@ -5968,9 +6351,9 @@
       <c r="N37" s="11">
         <v>0.97</v>
       </c>
-      <c r="O37" s="18"/>
-      <c r="P37" s="18"/>
-      <c r="Q37" s="18"/>
+      <c r="O37" s="43"/>
+      <c r="P37" s="43"/>
+      <c r="Q37" s="43"/>
     </row>
     <row r="38" spans="1:17">
       <c r="A38" s="1">
@@ -6244,16 +6627,16 @@
     </row>
     <row r="43" spans="1:17">
       <c r="B43" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H43" s="1">
         <v>1</v>
@@ -6261,16 +6644,16 @@
     </row>
     <row r="44" spans="1:17">
       <c r="B44" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H44" s="1">
         <v>1</v>
@@ -6278,16 +6661,16 @@
     </row>
     <row r="45" spans="1:17">
       <c r="B45" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H45" s="1">
         <v>1</v>
@@ -6295,16 +6678,16 @@
     </row>
     <row r="46" spans="1:17">
       <c r="B46" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H46" s="1">
         <v>1</v>
@@ -6312,16 +6695,16 @@
     </row>
     <row r="47" spans="1:17">
       <c r="B47" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H47" s="1">
         <v>1</v>
@@ -6329,16 +6712,16 @@
     </row>
     <row r="48" spans="1:17">
       <c r="B48" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H48" s="1">
         <v>1</v>
@@ -6346,16 +6729,16 @@
     </row>
     <row r="49" spans="2:8">
       <c r="B49" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H49" s="1">
         <v>1</v>
@@ -6363,16 +6746,16 @@
     </row>
     <row r="50" spans="2:8">
       <c r="B50" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H50" s="1">
         <v>1</v>
@@ -6380,7 +6763,7 @@
     </row>
     <row r="51" spans="2:8">
       <c r="B51" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>81</v>
@@ -6389,7 +6772,7 @@
         <v>23</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H51" s="1">
         <v>1</v>
@@ -6397,7 +6780,7 @@
     </row>
     <row r="52" spans="2:8">
       <c r="B52" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>81</v>
@@ -6406,7 +6789,7 @@
         <v>23</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H52" s="1">
         <v>1</v>
@@ -6414,7 +6797,7 @@
     </row>
     <row r="53" spans="2:8">
       <c r="B53" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>81</v>
@@ -6423,20 +6806,32 @@
         <v>23</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H53" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="2:8">
-      <c r="B54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
+      <c r="B54" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H54" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="2:8">
       <c r="B55" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>81</v>
@@ -6453,15 +6848,15 @@
     </row>
     <row r="56" spans="2:8">
       <c r="B56" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="G56" s="44" t="s">
         <v>97</v>
       </c>
       <c r="H56" s="1">
@@ -6470,7 +6865,7 @@
     </row>
     <row r="57" spans="2:8">
       <c r="B57" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>82</v>
@@ -6478,7 +6873,7 @@
       <c r="F57" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G57" s="17" t="s">
+      <c r="G57" s="44" t="s">
         <v>98</v>
       </c>
       <c r="H57" s="1">
@@ -6487,7 +6882,7 @@
     </row>
     <row r="58" spans="2:8">
       <c r="B58" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>82</v>
@@ -6495,7 +6890,7 @@
       <c r="F58" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G58" s="17" t="s">
+      <c r="G58" s="44" t="s">
         <v>99</v>
       </c>
       <c r="H58" s="1">
@@ -6504,15 +6899,15 @@
     </row>
     <row r="59" spans="2:8">
       <c r="B59" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G59" s="17" t="s">
+      <c r="G59" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H59" s="1">
@@ -6520,85 +6915,53 @@
       </c>
     </row>
     <row r="60" spans="2:8">
-      <c r="B60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
+      <c r="B60" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H60" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="61" spans="2:8">
-      <c r="B61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
+      <c r="B61" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H61" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="62" spans="2:8">
-      <c r="B62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-    </row>
-    <row r="63" spans="2:8">
-      <c r="B63" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E63" s="1" t="s">
+      <c r="B62" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F62" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G63" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H63" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8">
-      <c r="B64" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H64" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="2:8">
-      <c r="B65" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G65" s="1" t="s">
+      <c r="G62" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H65" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="2:8">
-      <c r="B66" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H66" s="1">
+      <c r="H62" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SI figures and script updated and main analysis script file renamed
</commit_message>
<xml_diff>
--- a/doc/manuscript/Tables.xlsx
+++ b/doc/manuscript/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="38640" yWindow="2480" windowWidth="23040" windowHeight="17460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="8940" yWindow="680" windowWidth="23040" windowHeight="17460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="6" r:id="rId1"/>
@@ -1458,29 +1458,34 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1488,14 +1493,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="371">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -19209,24 +19209,24 @@
     <row r="2" spans="1:16382">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="56" t="s">
         <v>162</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
-      <c r="K2" s="64" t="s">
+      <c r="K2" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
@@ -35595,34 +35595,34 @@
       <c r="XFB2" s="12"/>
     </row>
     <row r="3" spans="1:16382">
-      <c r="C3" s="60">
+      <c r="C3" s="57">
         <v>2011</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60">
+      <c r="D3" s="57"/>
+      <c r="E3" s="57">
         <v>2019</v>
       </c>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60" t="s">
+      <c r="F3" s="57"/>
+      <c r="G3" s="57" t="s">
         <v>163</v>
       </c>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60" t="s">
+      <c r="H3" s="57"/>
+      <c r="I3" s="57" t="s">
         <v>164</v>
       </c>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60" t="s">
+      <c r="J3" s="57"/>
+      <c r="K3" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60" t="s">
+      <c r="L3" s="57"/>
+      <c r="M3" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="60"/>
-      <c r="O3" s="65" t="s">
+      <c r="N3" s="57"/>
+      <c r="O3" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="P3" s="65"/>
+      <c r="P3" s="60"/>
     </row>
     <row r="4" spans="1:16382">
       <c r="A4" s="33" t="s">
@@ -35677,12 +35677,12 @@
     <row r="5" spans="1:16382" ht="16">
       <c r="A5" s="2"/>
       <c r="B5" s="34"/>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="58" t="s">
         <v>161</v>
       </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
       <c r="G5" s="59" t="s">
         <v>40</v>
       </c>
@@ -35986,7 +35986,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -36013,12 +36013,12 @@
       <c r="D2" s="19"/>
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="54" t="s">
+      <c r="G2" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
     </row>
     <row r="3" spans="1:10">
       <c r="B3" s="20"/>
@@ -36026,14 +36026,14 @@
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54" t="s">
+      <c r="H3" s="62"/>
+      <c r="I3" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="54"/>
+      <c r="J3" s="62"/>
     </row>
     <row r="4" spans="1:10" ht="45" customHeight="1">
       <c r="A4" s="22" t="s">
@@ -36100,7 +36100,7 @@
       <c r="J6" s="23"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="55">
+      <c r="A7" s="61">
         <v>1</v>
       </c>
       <c r="B7" s="36" t="s">
@@ -36133,7 +36133,7 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="55"/>
+      <c r="A8" s="61"/>
       <c r="B8" s="36" t="s">
         <v>11</v>
       </c>
@@ -36163,7 +36163,7 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="55">
+      <c r="A9" s="61">
         <v>2</v>
       </c>
       <c r="B9" s="36" t="s">
@@ -36196,7 +36196,7 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="55"/>
+      <c r="A10" s="61"/>
       <c r="B10" s="36" t="s">
         <v>13</v>
       </c>
@@ -36226,7 +36226,7 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="55">
+      <c r="A11" s="61">
         <v>3</v>
       </c>
       <c r="B11" s="36" t="s">
@@ -36258,7 +36258,7 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="55"/>
+      <c r="A12" s="61"/>
       <c r="B12" s="36" t="s">
         <v>11</v>
       </c>
@@ -36336,7 +36336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -36359,7 +36359,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="55" t="s">
         <v>183</v>
       </c>
     </row>
@@ -36369,19 +36369,19 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57" t="s">
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
       <c r="O2" s="29"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1">
@@ -36390,23 +36390,23 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="61" t="s">
+      <c r="F3" s="63" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="63" t="s">
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="J3" s="63"/>
-      <c r="K3" s="61" t="s">
+      <c r="J3" s="66"/>
+      <c r="K3" s="63" t="s">
         <v>135</v>
       </c>
-      <c r="L3" s="61"/>
-      <c r="M3" s="63" t="s">
+      <c r="L3" s="63"/>
+      <c r="M3" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="N3" s="63"/>
+      <c r="N3" s="66"/>
     </row>
     <row r="4" spans="1:15" ht="30" customHeight="1">
       <c r="A4" s="43" t="s">
@@ -36458,17 +36458,17 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="62" t="s">
+      <c r="F5" s="65" t="s">
         <v>140</v>
       </c>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1">
@@ -36859,8 +36859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -36895,21 +36895,21 @@
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
-      <c r="L2" s="57" t="s">
+      <c r="L2" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="M2" s="57"/>
+      <c r="M2" s="64"/>
       <c r="N2" s="14"/>
       <c r="O2" s="15"/>
       <c r="P2" s="15"/>
-      <c r="Q2" s="57" t="s">
+      <c r="Q2" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
+      <c r="R2" s="64"/>
+      <c r="S2" s="64"/>
     </row>
     <row r="3" spans="1:22" ht="45">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="54" t="s">
         <v>131</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -36951,10 +36951,10 @@
       <c r="N3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="O3" s="60" t="s">
+      <c r="O3" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="P3" s="60"/>
+      <c r="P3" s="57"/>
       <c r="Q3" s="4" t="s">
         <v>39</v>
       </c>
@@ -36991,10 +36991,10 @@
       <c r="K4" s="46" t="s">
         <v>172</v>
       </c>
-      <c r="L4" s="56" t="s">
+      <c r="L4" s="58" t="s">
         <v>130</v>
       </c>
-      <c r="M4" s="56"/>
+      <c r="M4" s="58"/>
       <c r="N4" s="6" t="s">
         <v>92</v>
       </c>
@@ -39947,12 +39947,12 @@
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="20"/>
@@ -39960,14 +39960,14 @@
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
-      <c r="F5" s="54" t="s">
+      <c r="F5" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54" t="s">
+      <c r="G5" s="62"/>
+      <c r="H5" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="54"/>
+      <c r="I5" s="62"/>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1">
       <c r="A6" s="21" t="s">
@@ -40122,12 +40122,12 @@
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
-      <c r="F13" s="54" t="s">
+      <c r="F13" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="20"/>
@@ -40135,14 +40135,14 @@
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
-      <c r="F14" s="54" t="s">
+      <c r="F14" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54" t="s">
+      <c r="G14" s="62"/>
+      <c r="H14" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="54"/>
+      <c r="I14" s="62"/>
     </row>
     <row r="15" spans="1:9" s="5" customFormat="1" ht="30" customHeight="1">
       <c r="A15" s="22" t="s">
@@ -40287,7 +40287,7 @@
   <dimension ref="A1:AC29"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -40308,39 +40308,39 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="57" t="s">
+      <c r="F2" s="64"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
       <c r="L2" s="32"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="57" t="s">
+      <c r="Q2" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="58"/>
+      <c r="R2" s="64"/>
+      <c r="S2" s="67"/>
       <c r="T2" s="32"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
-      <c r="W2" s="58"/>
+      <c r="U2" s="67"/>
+      <c r="V2" s="67"/>
+      <c r="W2" s="67"/>
       <c r="X2" s="32"/>
-      <c r="Y2" s="57" t="s">
+      <c r="Y2" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="57"/>
-      <c r="AC2" s="58"/>
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="64"/>
+      <c r="AB2" s="64"/>
+      <c r="AC2" s="67"/>
     </row>
     <row r="3" spans="1:29">
       <c r="A3" s="3" t="s">
@@ -40385,10 +40385,10 @@
       <c r="D4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="56"/>
+      <c r="F4" s="58"/>
       <c r="G4" s="2" t="s">
         <v>40</v>
       </c>
@@ -40885,7 +40885,14 @@
       </c>
     </row>
     <row r="18" spans="1:16">
-      <c r="E18" s="38"/>
+      <c r="E18" s="38">
+        <f>_xlfn.STDEV.S(E6:E17)</f>
+        <v>10.263177369266291</v>
+      </c>
+      <c r="F18">
+        <f>_xlfn.STDEV.S(F12:F17)</f>
+        <v>2.4740757505760298</v>
+      </c>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="37" t="s">

</xml_diff>